<commit_message>
added 1 tc for bento to setup jenkins
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5BA1CE-DDB2-4B14-BAF5-CB9734444896}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60AB68C-8012-43F8-A309-6C0B43F621C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
bento test script working without neo4j
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60AB68C-8012-43F8-A309-6C0B43F621C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ECF0C5-26EE-4B96-880F-F7BBA181C2A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>TC01_Bento_Filter_Program-TailorX_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
   </si>
 </sst>
 </file>
@@ -424,45 +430,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="75.81640625" customWidth="1"/>
-    <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.81640625" customWidth="1"/>
+    <col min="3" max="3" width="128.54296875" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="43.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="174" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated for MGT01 Study Combination
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Bento_0301\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD6883D-0849-46C0-84DD-6A507C566EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3617DDF-BA53-4B91-BA98-15E4009AEB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -45,9 +45,6 @@
     <t>StatQuery</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Beagle']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>TC01_Bento_Filter_Program-TailorX_Neo4jData.xlsx</t>
   </si>
   <si>
@@ -55,13 +52,6 @@
   </si>
   <si>
     <t>TabName</t>
-  </si>
-  <si>
-    <t>CasesTab</t>
-  </si>
-  <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['Beagle'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`
- order By ss.study_subject_id ASC LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -82,26 +72,33 @@
 COUNT(DISTINCT f) AS Files</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (ss:study_subject)
+    <t>MATCH (ss:study_subject)
+Match (s:study)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, 
+collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, 
+collect(DISTINCT f) AS files
+MATCH (s)-[:study_of_program]-&gt;(p)
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+OPTIONAL MATCH (ss)&lt;-[:program_of_institution]-(p)
+OPTIONAL MATCH (p)&lt;-[:of_arm]-(a)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
 MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE p.program_acronym IN ["TAILORx"]  
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`  order By ss.study_subject_id ASC LIMIT 100 </t>
+RETURN DISTINCT
+       coalesce (p.program_acronym, '')as `Program Code`,
+       coalesce( p.program_id , '')as Program_ID,
+       coalesce (p.program_name , '' )as `Program Name`,
+       coalesce(p.start_date, '') as `Start Date`,
+       coalesce (p.end_date, '') as `End Date`,
+       coalesce(p.pubmed_id, '') as `PubMed ID`,
+       count(distinct s) As `Number of Arms`,
+       count(distinct ss) as `Associated Cases`
+       order By `Program Code`</t>
+  </si>
+  <si>
+    <t>Casestab</t>
   </si>
 </sst>
 </file>
@@ -474,21 +471,21 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -503,30 +500,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
MGT01 Study comb 14to25
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\Bento_0301\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0302\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3617DDF-BA53-4B91-BA98-15E4009AEB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35762B2B-663D-43EA-9DF7-F8B693CCDCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D0644CC-C163-4BC0-BB31-C0CEB1B1B0C6}"/>
   </bookViews>
   <sheets>
-    <sheet name="startup" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,43 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>StatQuery</t>
+  </si>
+  <si>
+    <t>dbExcel</t>
+  </si>
+  <si>
     <t>WebExcel</t>
-  </si>
-  <si>
-    <t>query</t>
-  </si>
-  <si>
-    <t>dbExcel</t>
-  </si>
-  <si>
-    <t>StatQuery</t>
-  </si>
-  <si>
-    <t>TC01_Bento_Filter_Program-TailorX_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_Bento_Filter_Program-TailorX_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>TabName</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)  
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
-MATCH (samp)&lt;-[:file_of_sample]-(f)
-MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
-WHERE p.program_acronym IN ["TAILORx"]
-RETURN COUNT(DISTINCT p) AS Programs,
-COUNT(DISTINCT s) AS Arms,
-COUNT(DISTINCT ss) AS Cases,
-COUNT(DISTINCT samp) AS Samples,
-COUNT(DISTINCT lp) AS Assays,
-COUNT(DISTINCT f) AS Files</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -98,30 +79,41 @@
        order By `Program Code`</t>
   </si>
   <si>
-    <t>Casestab</t>
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)  
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+MATCH (samp)&lt;-[:file_of_sample]-(f)
+MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
+WHERE p.program_acronym IN ["TAILORx"]
+RETURN COUNT(DISTINCT p) AS Programs,
+COUNT(DISTINCT s) AS Arms,
+COUNT(DISTINCT ss) AS Cases,
+COUNT(DISTINCT samp) AS Samples,
+COUNT(DISTINCT lp) AS Assays,
+COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>Programstab</t>
+  </si>
+  <si>
+    <t>TC01_Bento_Filter_Program-TailorX_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_Bento_Filter_Program-TailorX_WebData.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,9 +136,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -154,9 +145,8 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{7EA68BB1-159D-4F44-96A3-D0B7FBE8815D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,63 +457,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B47B58B-CDB4-42B1-AF93-38CAEAF2792F}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" customWidth="1"/>
+    <col min="3" max="3" width="61" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="375" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="266.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NCATS Study multifilter testcases61to70
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0403\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD6883D-0849-46C0-84DD-6A507C566EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FF120E-466E-4076-BF16-37E714DDC07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="31080" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -45,9 +45,6 @@
     <t>StatQuery</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Beagle']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>TC01_Bento_Filter_Program-TailorX_Neo4jData.xlsx</t>
   </si>
   <si>
@@ -55,13 +52,6 @@
   </si>
   <si>
     <t>TabName</t>
-  </si>
-  <si>
-    <t>CasesTab</t>
-  </si>
-  <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['Beagle'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`
- order By ss.study_subject_id ASC LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -82,26 +72,33 @@
 COUNT(DISTINCT f) AS Files</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (ss:study_subject)
+    <t>MATCH (ss:study_subject)
+Match (s:study)
 MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, 
+collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, 
+collect(DISTINCT f) AS files
+MATCH (s)-[:study_of_program]-&gt;(p)
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+OPTIONAL MATCH (ss)&lt;-[:program_of_institution]-(p)
+OPTIONAL MATCH (p)&lt;-[:of_arm]-(a)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
 MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE p.program_acronym IN ["TAILORx"]  
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`  order By ss.study_subject_id ASC LIMIT 100 </t>
+RETURN DISTINCT
+       coalesce (p.program_acronym, '')as `Program Code`,
+       coalesce( p.program_id , '')as `Program ID`,
+       coalesce (p.program_name , '' )as `Program Name`,
+       coalesce(p.start_date, '') as `Start Date`,
+       coalesce (p.end_date, '') as `End Date`,
+       coalesce(p.pubmed_id, '') as `PubMed ID`,
+       count(distinct s) As `Number of Arms`,
+       count(distinct ss) as `Associated Cases`
+       order By `Program Code`</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
   </si>
 </sst>
 </file>
@@ -471,24 +468,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -503,29 +500,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="259.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bento Programs page is working.All issues haven resolved.Bento Profiles(Dev,QA,PERF and PROD) have been modified accordingly.
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Program-TailorX.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0403\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0413\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FF120E-466E-4076-BF16-37E714DDC07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D79310-C286-4281-BE3D-8F53DDDAE446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31080" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,6 +71,9 @@
 COUNT(DISTINCT samp) AS Samples,
 COUNT(DISTINCT lp) AS Assays,
 COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>ProgramsTab</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -92,13 +96,10 @@
        coalesce (p.program_name , '' )as `Program Name`,
        coalesce(p.start_date, '') as `Start Date`,
        coalesce (p.end_date, '') as `End Date`,
-       coalesce(p.pubmed_id, '') as `PubMed ID`,
+      coalesce(p.pubmed_id, '') as `PubMed ID`,
        count(distinct s) As `Number of Arms`,
        count(distinct ss) as `Associated Cases`
        order By `Program Code`</t>
-  </si>
-  <si>
-    <t>CasesTab</t>
   </si>
 </sst>
 </file>
@@ -471,7 +472,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +503,10 @@
     </row>
     <row r="2" spans="1:5" ht="259.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>

</xml_diff>